<commit_message>
add multiresolution Sioux Falls networks
</commit_message>
<xml_diff>
--- a/Sioux_Falls/summary.xlsx
+++ b/Sioux_Falls/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18016\Documents\GitHub\gmns_education_data_sets\Sioux_Falls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521A5513-1BB7-497A-B292-CA3D15E401E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B982642D-14B4-42B5-86BE-7723C01040B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5772" yWindow="3120" windowWidth="17280" windowHeight="9960" xr2:uid="{2DA63460-D9BE-40DB-8ECC-AB5409A44447}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="9960" xr2:uid="{2DA63460-D9BE-40DB-8ECC-AB5409A44447}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,12 +439,14 @@
   <dimension ref="A3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -564,5 +566,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>